<commit_message>
graph changes, nested loop is made explicit
</commit_message>
<xml_diff>
--- a/results/VIGraphs.xlsx
+++ b/results/VIGraphs.xlsx
@@ -332,7 +332,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.126060507606452"/>
+          <c:y val="0.0510816762311491"/>
+          <c:w val="0.842386094335295"/>
+          <c:h val="0.869822278571111"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -566,11 +576,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2051371720"/>
-        <c:axId val="2057814408"/>
+        <c:axId val="2106375464"/>
+        <c:axId val="2106381192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2051371720"/>
+        <c:axId val="2106375464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -587,7 +597,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Different</a:t>
+                  <a:t>different</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
@@ -604,7 +614,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2057814408"/>
+        <c:crossAx val="2106381192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -612,7 +622,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2057814408"/>
+        <c:axId val="2106381192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -646,14 +656,23 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2051371720"/>
+        <c:crossAx val="2106375464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.292397943582295"/>
+          <c:y val="0.189265536723164"/>
+          <c:w val="0.250155378029203"/>
+          <c:h val="0.0567313937452734"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -699,7 +718,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11777081436249"/>
+          <c:y val="0.0479857117579404"/>
+          <c:w val="0.852750727587623"/>
+          <c:h val="0.873362602848801"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -816,15 +845,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>all!$L$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>amltwenty</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>aml*</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cmpd="sng"/>
@@ -1360,11 +1381,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2059753304"/>
-        <c:axId val="2056141128"/>
+        <c:axId val="2106429816"/>
+        <c:axId val="2106435480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2059753304"/>
+        <c:axId val="2106429816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1381,7 +1402,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Different parameter sets</a:t>
+                  <a:t>different parameter sets</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1392,7 +1413,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2056141128"/>
+        <c:crossAx val="2106435480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1400,7 +1421,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2056141128"/>
+        <c:axId val="2106435480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1429,14 +1450,23 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2059753304"/>
+        <c:crossAx val="2106429816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.179526487760458"/>
+          <c:y val="0.0449438202247191"/>
+          <c:w val="0.432330244433731"/>
+          <c:h val="0.210907060072547"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1472,7 +1502,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0976743903708071"/>
+          <c:y val="0.0548359580052493"/>
+          <c:w val="0.873691248395713"/>
+          <c:h val="0.864704271879808"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1589,15 +1629,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>all!$U$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>amltwenty</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>aml*</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cmpd="sng"/>
@@ -2030,11 +2062,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2059578344"/>
-        <c:axId val="2058543416"/>
+        <c:axId val="2106475688"/>
+        <c:axId val="2106481416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2059578344"/>
+        <c:axId val="2106475688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2051,7 +2083,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Different parameter sets</a:t>
+                  <a:t>different parameter sets</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2062,7 +2094,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2058543416"/>
+        <c:crossAx val="2106481416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2070,7 +2102,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2058543416"/>
+        <c:axId val="2106481416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2099,14 +2131,23 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2059578344"/>
+        <c:crossAx val="2106475688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.142958479309029"/>
+          <c:y val="0.0316091954022988"/>
+          <c:w val="0.377078462659128"/>
+          <c:h val="0.215755498235134"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2142,7 +2183,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0966103991902973"/>
+          <c:y val="0.0405847648006535"/>
+          <c:w val="0.875067160722557"/>
+          <c:h val="0.87872359254805"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -2259,15 +2310,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>all!$AD$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>amltwenty</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>aml*</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cmpd="sng"/>
@@ -2700,11 +2743,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2057989864"/>
-        <c:axId val="2059568392"/>
+        <c:axId val="2106522904"/>
+        <c:axId val="2106528888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2057989864"/>
+        <c:axId val="2106522904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2721,7 +2764,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Different parameter</a:t>
+                  <a:t>different parameter</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
@@ -2737,7 +2780,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2059568392"/>
+        <c:crossAx val="2106528888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2745,7 +2788,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2059568392"/>
+        <c:axId val="2106528888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2762,7 +2805,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Accuracy (VI score)</a:t>
+                  <a:t>accuracy (VI score)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2774,14 +2817,23 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2057989864"/>
+        <c:crossAx val="2106522904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.164277014392809"/>
+          <c:y val="0.0288184438040346"/>
+          <c:w val="0.394757346508157"/>
+          <c:h val="0.210613583244458"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2807,8 +2859,8 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -2931,7 +2983,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="nu100" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ESvES2" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2939,7 +2991,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ESvES2" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="nu100" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3266,8 +3318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:AG41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="Y39" sqref="Y39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>